<commit_message>
fixed typo in traps input data
</commit_message>
<xml_diff>
--- a/data/traps/LiveOcean_SSM_rivers.xlsx
+++ b/data/traps/LiveOcean_SSM_rivers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\aleeson\LO_data\traps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C883D2-DA66-40B7-865F-681B2504386E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05597360-A774-4EBD-BA96-FC8DDA3FE9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F487C1D6-8DE6-4428-AAF5-0A5909261804}"/>
+    <workbookView xWindow="22932" yWindow="1920" windowWidth="23256" windowHeight="12456" xr2:uid="{F487C1D6-8DE6-4428-AAF5-0A5909261804}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>coquille</t>
   </si>
   <si>
-    <t xml:space="preserve">Fraser R </t>
-  </si>
-  <si>
     <t>Nooksack R</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>Capitol Lake</t>
+  </si>
+  <si>
+    <t>Fraser R</t>
   </si>
 </sst>
 </file>
@@ -627,8 +627,8 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,16 +641,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -661,10 +661,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,10 +798,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -955,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>